<commit_message>
Set correct failure mechanism name in acceptance test files. ASK-87
</commit_message>
<xml_diff>
--- a/test/Assembly.Kernel.Acceptance.Test/test-data/definitions/Benchmarktest_traject 13-2.xlsx
+++ b/test/Assembly.Kernel.Acceptance.Test/test-data/definitions/Benchmarktest_traject 13-2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Checkouts\AssemblageKernel\test\Assembly.Kernel.Acceptance.Test\test-data\definitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9174DFB-D630-4ECC-AF0B-9F9666AD3777}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D692B1C6-CAAF-4F28-838F-6FBCD0E435C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="9" xr2:uid="{0831170E-5124-493D-8FBC-5E58312EFD65}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{0831170E-5124-493D-8FBC-5E58312EFD65}"/>
   </bookViews>
   <sheets>
     <sheet name="Informatiepagina" sheetId="1" r:id="rId1"/>
@@ -267,9 +267,6 @@
     <t>Macrostabiliteit</t>
   </si>
   <si>
-    <t>Erosie van het buitentalud</t>
-  </si>
-  <si>
     <t>Duinafslag</t>
   </si>
   <si>
@@ -502,6 +499,9 @@
   </si>
   <si>
     <t>Gecorreleerd</t>
+  </si>
+  <si>
+    <t>Erosie van het binnentalud</t>
   </si>
 </sst>
 </file>
@@ -1027,20 +1027,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="darkUp">
           <fgColor theme="0"/>
           <bgColor rgb="FFFF0000"/>
@@ -1059,6 +1045,20 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1185,6 +1185,20 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="darkUp">
           <fgColor theme="0"/>
           <bgColor rgb="FFFF0000"/>
@@ -1203,20 +1217,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1990,19 +1990,19 @@
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="D2" s="48" t="s">
+      <c r="E2" s="48" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="49" t="s">
         <v>91</v>
-      </c>
-      <c r="E2" s="48" t="s">
-        <v>101</v>
-      </c>
-      <c r="F2" s="49" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -2010,7 +2010,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>28</v>
@@ -2027,7 +2027,7 @@
         <v>73</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>28</v>
@@ -2041,10 +2041,10 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>29</v>
@@ -2053,21 +2053,21 @@
         <v>28</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>29</v>
@@ -2075,16 +2075,16 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>29</v>
@@ -2092,10 +2092,10 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>29</v>
@@ -2109,16 +2109,16 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>29</v>
@@ -2126,16 +2126,16 @@
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>29</v>
@@ -2143,10 +2143,10 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>29</v>
@@ -2160,10 +2160,10 @@
     </row>
     <row r="12" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>106</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>107</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>29</v>
@@ -2172,7 +2172,7 @@
         <v>29</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2223,7 +2223,7 @@
   </sheetPr>
   <dimension ref="B2:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -2243,7 +2243,7 @@
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" s="1">
         <f>IFERROR(1-PRODUCT(M7:M13)*(1-L15),"GR")</f>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D3" s="1">
         <f>1-PRODUCT(O7:O13)*(1-N15)</f>
@@ -2297,39 +2297,39 @@
         <v>49</v>
       </c>
       <c r="E6" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F6" s="45" t="s">
-        <v>152</v>
-      </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="J6" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7" s="29">
         <f>STPH!C7</f>
@@ -2379,7 +2379,7 @@
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" s="31">
         <f>STBI!C7</f>
@@ -2429,7 +2429,7 @@
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" s="31">
         <f>GEKB!C7</f>
@@ -2479,7 +2479,7 @@
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" s="31">
         <f>DA!C7</f>
@@ -2529,7 +2529,7 @@
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="31">
         <f>STKWp!C7</f>
@@ -2579,7 +2579,7 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" s="31">
         <f>HTKW!C7</f>
@@ -2629,7 +2629,7 @@
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="40" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C13" s="31">
         <f>BSKW!C7</f>
@@ -2688,7 +2688,7 @@
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I15" s="1"/>
       <c r="K15" s="1"/>
@@ -2792,31 +2792,31 @@
       <c r="B2" s="9"/>
       <c r="C2" s="14"/>
       <c r="D2" s="63" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E2" s="63" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F2" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="48" t="s">
+      <c r="H2" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="48" t="s">
+      <c r="I2" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="I2" s="48" t="s">
+      <c r="J2" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="J2" s="48" t="s">
+      <c r="K2" s="48" t="s">
+        <v>99</v>
+      </c>
+      <c r="L2" s="49" t="s">
         <v>80</v>
-      </c>
-      <c r="K2" s="48" t="s">
-        <v>100</v>
-      </c>
-      <c r="L2" s="49" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
@@ -5466,7 +5466,7 @@
         <v>60</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>48</v>
@@ -5511,7 +5511,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B5" s="9">
         <v>5.7050000000000001</v>
@@ -5568,12 +5568,12 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D11" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D12" s="47" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E12" s="49" t="s">
         <v>47</v>
@@ -5729,7 +5729,7 @@
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B4" s="40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>28</v>
@@ -5737,15 +5737,15 @@
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B5" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>136</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B6" s="40" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>29</v>
@@ -5780,7 +5780,7 @@
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B10" s="40" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C10" s="26">
         <f>MAX(Z16:Z35)</f>
@@ -5798,7 +5798,7 @@
     </row>
     <row r="12" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C12" s="27">
         <f>1-PRODUCT(R16:R35)</f>
@@ -5818,7 +5818,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E15" s="21" t="s">
         <v>3</v>
@@ -5877,10 +5877,10 @@
         <v>71</v>
       </c>
       <c r="Y15" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z15" s="39" t="s">
         <v>140</v>
-      </c>
-      <c r="Z15" s="39" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="16" spans="2:26" x14ac:dyDescent="0.25">
@@ -6621,7 +6621,7 @@
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B4" s="40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>28</v>
@@ -6629,15 +6629,15 @@
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B5" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>136</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B6" s="40" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>29</v>
@@ -6672,7 +6672,7 @@
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B10" s="40" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C10" s="26">
         <f>MAX(Z16:Z35)</f>
@@ -6690,7 +6690,7 @@
     </row>
     <row r="12" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C12" s="27">
         <f>1-PRODUCT(R16:R35)</f>
@@ -6710,7 +6710,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E15" s="21" t="s">
         <v>3</v>
@@ -6769,10 +6769,10 @@
         <v>71</v>
       </c>
       <c r="Y15" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z15" s="39" t="s">
         <v>142</v>
-      </c>
-      <c r="Z15" s="39" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="16" spans="2:26" x14ac:dyDescent="0.25">
@@ -7471,8 +7471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E4BDF32-8A22-4A66-B6B5-DB37648E7DC4}">
   <dimension ref="B2:V78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7496,7 +7496,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>74</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
@@ -7509,7 +7509,7 @@
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>29</v>
@@ -7517,15 +7517,15 @@
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>136</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="40" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>29</v>
@@ -7560,7 +7560,7 @@
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" s="40" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C10" s="26">
         <f>MAX(V16:V76)</f>
@@ -7578,7 +7578,7 @@
     </row>
     <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C12" s="27">
         <f>1-PRODUCT(N16:N76)</f>
@@ -7629,10 +7629,10 @@
         <v>51</v>
       </c>
       <c r="O15" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="P15" s="37" t="s">
         <v>88</v>
-      </c>
-      <c r="P15" s="37" t="s">
-        <v>89</v>
       </c>
       <c r="Q15" s="38" t="s">
         <v>69</v>
@@ -7645,15 +7645,15 @@
         <v>71</v>
       </c>
       <c r="U15" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="V15" s="39" t="s">
         <v>142</v>
-      </c>
-      <c r="V15" s="39" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C16" s="4">
         <v>0</v>
@@ -9189,7 +9189,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
@@ -9202,7 +9202,7 @@
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>29</v>
@@ -9210,15 +9210,15 @@
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="40" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="40" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>29</v>
@@ -9253,7 +9253,7 @@
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" s="40" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C10" s="26">
         <f>MAX(V16:V55)</f>
@@ -9271,7 +9271,7 @@
     </row>
     <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C12" s="27">
         <f>1-PRODUCT(N16:N55)</f>
@@ -9338,10 +9338,10 @@
         <v>71</v>
       </c>
       <c r="U15" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="V15" s="39" t="s">
         <v>140</v>
-      </c>
-      <c r="V15" s="39" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
@@ -10806,7 +10806,7 @@
     </row>
     <row r="36" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B36" s="76" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C36" s="73">
         <v>3.302</v>
@@ -10879,7 +10879,7 @@
     </row>
     <row r="37" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B37" s="76" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C37" s="73">
         <v>3.4630000000000001</v>
@@ -10952,7 +10952,7 @@
     </row>
     <row r="38" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B38" s="76" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C38" s="73">
         <v>3.5960000000000001</v>
@@ -11025,7 +11025,7 @@
     </row>
     <row r="39" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B39" s="76" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C39" s="73">
         <v>3.726</v>
@@ -11098,7 +11098,7 @@
     </row>
     <row r="40" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B40" s="76" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C40" s="73">
         <v>3.8559999999999999</v>
@@ -11171,7 +11171,7 @@
     </row>
     <row r="41" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B41" s="76" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C41" s="73">
         <v>3.9809999999999999</v>
@@ -11244,7 +11244,7 @@
     </row>
     <row r="42" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B42" s="76" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C42" s="73">
         <v>4.1050000000000004</v>
@@ -11317,7 +11317,7 @@
     </row>
     <row r="43" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B43" s="76" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C43" s="73">
         <v>4.2359999999999998</v>
@@ -11390,7 +11390,7 @@
     </row>
     <row r="44" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B44" s="76" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C44" s="73">
         <v>4.38</v>
@@ -11463,7 +11463,7 @@
     </row>
     <row r="45" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B45" s="76" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C45" s="73">
         <v>4.5129999999999999</v>
@@ -11536,7 +11536,7 @@
     </row>
     <row r="46" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B46" s="76" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C46" s="73">
         <v>4.6340000000000003</v>
@@ -11609,7 +11609,7 @@
     </row>
     <row r="47" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B47" s="76" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C47" s="73">
         <v>4.7480000000000002</v>
@@ -11682,7 +11682,7 @@
     </row>
     <row r="48" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B48" s="76" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C48" s="73">
         <v>4.8609999999999998</v>
@@ -11755,7 +11755,7 @@
     </row>
     <row r="49" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B49" s="76" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C49" s="73">
         <v>4.9749999999999996</v>
@@ -11828,7 +11828,7 @@
     </row>
     <row r="50" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B50" s="76" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C50" s="73">
         <v>5.0910000000000002</v>
@@ -11901,7 +11901,7 @@
     </row>
     <row r="51" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B51" s="76" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C51" s="73">
         <v>5.2140000000000004</v>
@@ -11974,7 +11974,7 @@
     </row>
     <row r="52" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B52" s="76" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C52" s="73">
         <v>5.3390000000000004</v>
@@ -12047,7 +12047,7 @@
     </row>
     <row r="53" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B53" s="76" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C53" s="73">
         <v>5.4950000000000001</v>
@@ -12388,7 +12388,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
@@ -12401,7 +12401,7 @@
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>29</v>
@@ -12409,15 +12409,15 @@
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>136</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="40" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>29</v>
@@ -12452,7 +12452,7 @@
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" s="40" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C10" s="26">
         <f>MAX(V16:V33)</f>
@@ -12470,7 +12470,7 @@
     </row>
     <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C12" s="27">
         <f>1-PRODUCT(N16:N33)</f>
@@ -12521,10 +12521,10 @@
         <v>51</v>
       </c>
       <c r="O15" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="P15" s="37" t="s">
         <v>88</v>
-      </c>
-      <c r="P15" s="37" t="s">
-        <v>89</v>
       </c>
       <c r="Q15" s="38" t="s">
         <v>69</v>
@@ -12537,10 +12537,10 @@
         <v>71</v>
       </c>
       <c r="U15" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="V15" s="39" t="s">
         <v>140</v>
-      </c>
-      <c r="V15" s="39" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
@@ -13134,7 +13134,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
@@ -13147,7 +13147,7 @@
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>29</v>
@@ -13155,15 +13155,15 @@
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>136</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="40" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>29</v>
@@ -13198,7 +13198,7 @@
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" s="40" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C10" s="26">
         <f>MAX(V16:V32)</f>
@@ -13216,7 +13216,7 @@
     </row>
     <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C12" s="27">
         <f>1-PRODUCT(N16:N32)</f>
@@ -13271,10 +13271,10 @@
         <v>51</v>
       </c>
       <c r="O15" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="P15" s="37" t="s">
         <v>88</v>
-      </c>
-      <c r="P15" s="37" t="s">
-        <v>89</v>
       </c>
       <c r="Q15" s="38" t="s">
         <v>69</v>
@@ -13287,7 +13287,7 @@
         <v>71</v>
       </c>
       <c r="U15" s="38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="V15" s="39" t="s">
         <v>50</v>
@@ -13723,44 +13723,44 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G17:G20 G22:G32">
-    <cfRule type="expression" dxfId="26" priority="16">
+    <cfRule type="expression" dxfId="48" priority="16">
       <formula>IF($E17="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17:I32">
-    <cfRule type="expression" dxfId="25" priority="15">
+    <cfRule type="expression" dxfId="47" priority="15">
       <formula>IF($H17="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17:K32">
-    <cfRule type="cellIs" dxfId="24" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="12" operator="equal">
       <formula>"0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="13" operator="equal">
       <formula>"ND"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="14" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
       <formula>"0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
       <formula>"ND"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="3" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16">
-    <cfRule type="expression" dxfId="18" priority="5">
+    <cfRule type="expression" dxfId="40" priority="5">
       <formula>IF($E16="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="expression" dxfId="17" priority="4">
+    <cfRule type="expression" dxfId="39" priority="4">
       <formula>IF($H16="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13952,7 +13952,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
@@ -13965,7 +13965,7 @@
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>29</v>
@@ -13973,15 +13973,15 @@
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>136</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="40" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>29</v>
@@ -14016,7 +14016,7 @@
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" s="40" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C10" s="26">
         <f>MAX(V16:V33)</f>
@@ -14034,7 +14034,7 @@
     </row>
     <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C12" s="27">
         <f>1-PRODUCT(N16:N33)</f>
@@ -14089,10 +14089,10 @@
         <v>51</v>
       </c>
       <c r="O15" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="P15" s="37" t="s">
         <v>88</v>
-      </c>
-      <c r="P15" s="37" t="s">
-        <v>89</v>
       </c>
       <c r="Q15" s="38" t="s">
         <v>69</v>
@@ -14105,10 +14105,10 @@
         <v>71</v>
       </c>
       <c r="U15" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="V15" s="39" t="s">
         <v>140</v>
-      </c>
-      <c r="V15" s="39" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
@@ -14563,44 +14563,44 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G17:G33">
-    <cfRule type="expression" dxfId="48" priority="16">
+    <cfRule type="expression" dxfId="26" priority="16">
       <formula>IF($E17="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17:I33">
-    <cfRule type="expression" dxfId="47" priority="15">
+    <cfRule type="expression" dxfId="25" priority="15">
       <formula>IF($H17="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17:K33">
-    <cfRule type="cellIs" dxfId="46" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="12" operator="equal">
       <formula>"0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
       <formula>"ND"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="14" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16">
-    <cfRule type="expression" dxfId="43" priority="5">
+    <cfRule type="expression" dxfId="21" priority="5">
       <formula>IF($E16="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="expression" dxfId="42" priority="4">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>IF($H16="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16">
-    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
       <formula>"0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
       <formula>"ND"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>